<commit_message>
Made changes in classes
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/VRRLogistics/data/TestData.xlsx
+++ b/src/main/java/com/test/automation/VRRLogistics/data/TestData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12705" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>loginid</t>
   </si>
@@ -46,30 +46,6 @@
   </si>
   <si>
     <t>fffff</t>
-  </si>
-  <si>
-    <t>iftt</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>__12345</t>
-  </si>
-  <si>
-    <t>!#@@@</t>
-  </si>
-  <si>
-    <t>ssss</t>
-  </si>
-  <si>
-    <t>hhhhhhhhhhhhh</t>
-  </si>
-  <si>
-    <t>12!@#ff</t>
-  </si>
-  <si>
-    <t>32243!@@!@</t>
   </si>
 </sst>
 </file>
@@ -415,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,83 +438,6 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>13123424234</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed issues in datasheet
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/VRRLogistics/data/TestData.xlsx
+++ b/src/main/java/com/test/automation/VRRLogistics/data/TestData.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13215" windowHeight="10335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -120,8 +120,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,91 +460,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C10"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>